<commit_message>
changed bt not reflected
</commit_message>
<xml_diff>
--- a/Interview preparation.xlsx
+++ b/Interview preparation.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="278">
   <si>
     <t>Topics</t>
   </si>
@@ -2109,6 +2109,10 @@
   </si>
   <si>
     <t>Always start with Upper Case &amp; both should be the same name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ </t>
   </si>
 </sst>
 </file>
@@ -2855,6 +2859,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2953,9 +2960,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2995,7 +2999,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F0687AC-5F95-B371-FCC3-516ECEBB7F8D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4F0687AC-5F95-B371-FCC3-516ECEBB7F8D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3039,7 +3043,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38596EE9-12E8-E05D-656B-7E6C83468E69}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{38596EE9-12E8-E05D-656B-7E6C83468E69}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3083,7 +3087,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A44838A8-315A-6F11-F425-7C24684925CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A44838A8-315A-6F11-F425-7C24684925CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3127,7 +3131,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6468BF38-FF2D-C7D2-9142-120CFAF41A38}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6468BF38-FF2D-C7D2-9142-120CFAF41A38}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3171,7 +3175,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBCAADE1-0A65-E2AB-42C9-C833CC10A99A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EBCAADE1-0A65-E2AB-42C9-C833CC10A99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3219,7 +3223,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9A655E8-006A-EE32-F2F1-5080EB63AAF6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E9A655E8-006A-EE32-F2F1-5080EB63AAF6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3263,7 +3267,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA5A8967-9D46-7B4A-81EA-E5E7E0FBD1D4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FA5A8967-9D46-7B4A-81EA-E5E7E0FBD1D4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3307,7 +3311,7 @@
         <xdr:cNvPr id="10" name="Picture 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5628D44-680D-FB5E-E6FA-ECBA9934C1EE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D5628D44-680D-FB5E-E6FA-ECBA9934C1EE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3351,7 +3355,7 @@
         <xdr:cNvPr id="11" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7253AB4-994D-87AA-50A4-1E642115AF54}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E7253AB4-994D-87AA-50A4-1E642115AF54}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3395,7 +3399,7 @@
         <xdr:cNvPr id="12" name="Picture 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DDCCF8C-2871-9944-4A9D-EC8901C1674D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0DDCCF8C-2871-9944-4A9D-EC8901C1674D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3439,7 +3443,7 @@
         <xdr:cNvPr id="13" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D1A4CDE-62F4-A369-6F02-86865D0E6B72}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3D1A4CDE-62F4-A369-6F02-86865D0E6B72}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3488,7 +3492,7 @@
         <xdr:cNvPr id="2" name="Right Brace 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{271A39DF-730C-44C5-B2C6-BCC2EFAE8626}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{271A39DF-730C-44C5-B2C6-BCC2EFAE8626}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3566,7 +3570,7 @@
         <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5A86CCB-9035-382C-CB17-968C40DFAB49}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A5A86CCB-9035-382C-CB17-968C40DFAB49}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3616,7 +3620,7 @@
         <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5123DE96-BC07-92D0-1AEA-823B40633BA9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5123DE96-BC07-92D0-1AEA-823B40633BA9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3669,7 +3673,7 @@
         <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79B9A0D3-4108-418B-8375-3FDACBDFFF37}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{79B9A0D3-4108-418B-8375-3FDACBDFFF37}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3722,7 +3726,7 @@
         <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1073A0F4-BF25-49FD-B619-5EC5F802F813}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1073A0F4-BF25-49FD-B619-5EC5F802F813}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3775,7 +3779,7 @@
         <xdr:cNvPr id="11" name="Straight Connector 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{696E1177-F678-B27D-E168-36FA4288F520}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{696E1177-F678-B27D-E168-36FA4288F520}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3825,7 +3829,7 @@
         <xdr:cNvPr id="15" name="Straight Connector 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE6952BA-250D-47A8-9B95-78E49C76026E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AE6952BA-250D-47A8-9B95-78E49C76026E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3875,7 +3879,7 @@
         <xdr:cNvPr id="17" name="Connector: Elbow 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C26EC763-551C-C4BE-9443-748B6D540788}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C26EC763-551C-C4BE-9443-748B6D540788}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3933,7 +3937,7 @@
         <xdr:cNvPr id="20" name="Connector: Elbow 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{551A7CBE-D3B6-4E61-B697-B078049DE0AA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{551A7CBE-D3B6-4E61-B697-B078049DE0AA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4199,7 +4203,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4234,7 +4238,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4462,10 +4466,10 @@
       <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="62" t="s">
+      <c r="D2" s="63" t="s">
         <v>3</v>
       </c>
     </row>
@@ -4473,8 +4477,8 @@
       <c r="B3" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="63"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="64"/>
     </row>
     <row r="4" spans="2:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="56">
@@ -4546,7 +4550,7 @@
       <c r="B10" s="11">
         <v>7</v>
       </c>
-      <c r="C10" s="64" t="s">
+      <c r="C10" s="65" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -4557,7 +4561,7 @@
       <c r="B11" s="2">
         <v>8</v>
       </c>
-      <c r="C11" s="65"/>
+      <c r="C11" s="66"/>
       <c r="D11" s="4" t="s">
         <v>18</v>
       </c>
@@ -4599,7 +4603,7 @@
       <c r="B15" s="2">
         <v>12</v>
       </c>
-      <c r="C15" s="66" t="s">
+      <c r="C15" s="67" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -4610,7 +4614,7 @@
       <c r="B16" s="2">
         <v>13</v>
       </c>
-      <c r="C16" s="66"/>
+      <c r="C16" s="67"/>
       <c r="D16" s="4" t="s">
         <v>25</v>
       </c>
@@ -4745,19 +4749,19 @@
       <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="67" t="s">
+      <c r="C2" s="68" t="s">
         <v>222</v>
       </c>
-      <c r="D2" s="67" t="s">
+      <c r="D2" s="68" t="s">
         <v>3</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="67" t="s">
+      <c r="I2" s="68" t="s">
         <v>221</v>
       </c>
-      <c r="J2" s="67" t="s">
+      <c r="J2" s="68" t="s">
         <v>3</v>
       </c>
     </row>
@@ -4765,13 +4769,13 @@
       <c r="B3" s="39" t="s">
         <v>206</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
       <c r="H3" s="39" t="s">
         <v>206</v>
       </c>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
@@ -4921,19 +4925,19 @@
       <c r="B17" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="67" t="s">
+      <c r="C17" s="68" t="s">
         <v>214</v>
       </c>
-      <c r="D17" s="67" t="s">
+      <c r="D17" s="68" t="s">
         <v>3</v>
       </c>
       <c r="H17" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I17" s="67" t="s">
+      <c r="I17" s="68" t="s">
         <v>227</v>
       </c>
-      <c r="J17" s="67" t="s">
+      <c r="J17" s="68" t="s">
         <v>3</v>
       </c>
     </row>
@@ -4941,13 +4945,13 @@
       <c r="B18" s="39" t="s">
         <v>206</v>
       </c>
-      <c r="C18" s="67"/>
-      <c r="D18" s="67"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="68"/>
       <c r="H18" s="39" t="s">
         <v>206</v>
       </c>
-      <c r="I18" s="67"/>
-      <c r="J18" s="67"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="68"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="2">
@@ -5099,10 +5103,10 @@
       <c r="B31" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C31" s="67" t="s">
+      <c r="C31" s="68" t="s">
         <v>233</v>
       </c>
-      <c r="D31" s="67" t="s">
+      <c r="D31" s="68" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5110,8 +5114,8 @@
       <c r="B32" s="39" t="s">
         <v>206</v>
       </c>
-      <c r="C32" s="67"/>
-      <c r="D32" s="67"/>
+      <c r="C32" s="68"/>
+      <c r="D32" s="68"/>
     </row>
     <row r="33" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B33" s="2">
@@ -5210,8 +5214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5509,11 +5513,11 @@
       </c>
     </row>
     <row r="28" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B28" s="93">
+      <c r="B28" s="60">
         <v>26</v>
       </c>
       <c r="C28" s="40" t="s">
-        <v>187</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -5544,10 +5548,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="71"/>
+      <c r="C3" s="72"/>
       <c r="D3" s="15" t="s">
         <v>69</v>
       </c>
@@ -5559,10 +5563,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="72"/>
+      <c r="C4" s="73"/>
       <c r="D4" s="2" t="s">
         <v>73</v>
       </c>
@@ -5574,16 +5578,16 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="74" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="64" t="s">
+      <c r="C5" s="65" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="68" t="s">
+      <c r="D5" s="69" t="s">
         <v>78</v>
       </c>
-      <c r="E5" s="68" t="s">
+      <c r="E5" s="69" t="s">
         <v>78</v>
       </c>
       <c r="F5" s="14" t="s">
@@ -5591,16 +5595,16 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="73"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
       <c r="F6" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B7" s="73"/>
+      <c r="B7" s="74"/>
       <c r="C7" s="14" t="s">
         <v>81</v>
       </c>
@@ -5615,7 +5619,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B8" s="73"/>
+      <c r="B8" s="74"/>
       <c r="C8" s="14" t="s">
         <v>85</v>
       </c>
@@ -5630,7 +5634,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="B9" s="73"/>
+      <c r="B9" s="74"/>
       <c r="C9" s="14" t="s">
         <v>89</v>
       </c>
@@ -5641,7 +5645,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="B10" s="73"/>
+      <c r="B10" s="74"/>
       <c r="C10" s="14" t="s">
         <v>91</v>
       </c>
@@ -5652,7 +5656,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="73"/>
+      <c r="B11" s="74"/>
       <c r="C11" s="14" t="s">
         <v>93</v>
       </c>
@@ -5665,10 +5669,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B12" s="70" t="s">
+      <c r="B12" s="71" t="s">
         <v>96</v>
       </c>
-      <c r="C12" s="70"/>
+      <c r="C12" s="71"/>
       <c r="D12" s="4" t="s">
         <v>97</v>
       </c>
@@ -5711,10 +5715,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="74"/>
+      <c r="C2" s="75"/>
     </row>
     <row r="3" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="30" t="s">
@@ -6098,10 +6102,10 @@
       <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="67" t="s">
+      <c r="C2" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="67" t="s">
+      <c r="D2" s="68" t="s">
         <v>3</v>
       </c>
     </row>
@@ -6109,8 +6113,8 @@
       <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
     </row>
     <row r="4" spans="2:5" ht="294.60000000000002" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
@@ -6161,7 +6165,7 @@
       <c r="B8" s="2">
         <v>5</v>
       </c>
-      <c r="C8" s="64" t="s">
+      <c r="C8" s="65" t="s">
         <v>33</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -6172,7 +6176,7 @@
       <c r="B9" s="2">
         <v>6</v>
       </c>
-      <c r="C9" s="65"/>
+      <c r="C9" s="66"/>
       <c r="D9" s="4" t="s">
         <v>36</v>
       </c>
@@ -6355,11 +6359,11 @@
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:13" s="49" customFormat="1" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="85" t="s">
         <v>240</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="87"/>
       <c r="E3" s="50"/>
       <c r="F3" s="50"/>
       <c r="G3" s="50"/>
@@ -6371,11 +6375,11 @@
       <c r="M3" s="50"/>
     </row>
     <row r="4" spans="1:13" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="87" t="s">
+      <c r="B4" s="88" t="s">
         <v>241</v>
       </c>
-      <c r="C4" s="88"/>
-      <c r="D4" s="89"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="90"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5" s="51"/>
@@ -6488,21 +6492,21 @@
       <c r="D26" s="52"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B27" s="78"/>
-      <c r="C27" s="79"/>
-      <c r="D27" s="80"/>
+      <c r="B27" s="79"/>
+      <c r="C27" s="80"/>
+      <c r="D27" s="81"/>
     </row>
     <row r="28" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="81"/>
-      <c r="C28" s="82"/>
-      <c r="D28" s="83"/>
+      <c r="B28" s="82"/>
+      <c r="C28" s="83"/>
+      <c r="D28" s="84"/>
     </row>
     <row r="29" spans="2:4" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B29" s="90" t="s">
+      <c r="B29" s="91" t="s">
         <v>242</v>
       </c>
-      <c r="C29" s="91"/>
-      <c r="D29" s="92"/>
+      <c r="C29" s="92"/>
+      <c r="D29" s="93"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" s="51"/>
@@ -6605,21 +6609,21 @@
       <c r="D49" s="52"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B50" s="78"/>
-      <c r="C50" s="79"/>
-      <c r="D50" s="80"/>
+      <c r="B50" s="79"/>
+      <c r="C50" s="80"/>
+      <c r="D50" s="81"/>
     </row>
     <row r="51" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="81"/>
-      <c r="C51" s="82"/>
-      <c r="D51" s="83"/>
+      <c r="B51" s="82"/>
+      <c r="C51" s="83"/>
+      <c r="D51" s="84"/>
     </row>
     <row r="52" spans="2:4" ht="24" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="75" t="s">
+      <c r="B52" s="76" t="s">
         <v>243</v>
       </c>
-      <c r="C52" s="76"/>
-      <c r="D52" s="77"/>
+      <c r="C52" s="77"/>
+      <c r="D52" s="78"/>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B53" s="51"/>
@@ -6722,26 +6726,26 @@
       <c r="D72" s="52"/>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B73" s="78"/>
-      <c r="C73" s="79"/>
-      <c r="D73" s="80"/>
+      <c r="B73" s="79"/>
+      <c r="C73" s="80"/>
+      <c r="D73" s="81"/>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B74" s="78"/>
-      <c r="C74" s="79"/>
-      <c r="D74" s="80"/>
+      <c r="B74" s="79"/>
+      <c r="C74" s="80"/>
+      <c r="D74" s="81"/>
     </row>
     <row r="75" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B75" s="81"/>
-      <c r="C75" s="82"/>
-      <c r="D75" s="83"/>
+      <c r="B75" s="82"/>
+      <c r="C75" s="83"/>
+      <c r="D75" s="84"/>
     </row>
     <row r="76" spans="2:4" ht="24" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B76" s="75" t="s">
+      <c r="B76" s="76" t="s">
         <v>244</v>
       </c>
-      <c r="C76" s="76"/>
-      <c r="D76" s="77"/>
+      <c r="C76" s="77"/>
+      <c r="D76" s="78"/>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B77" s="51"/>

</xml_diff>

<commit_message>
Added some Ques & Ans
</commit_message>
<xml_diff>
--- a/Interview preparation.xlsx
+++ b/Interview preparation.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867D0A40-9118-4E9B-ACE7-6F8985363704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="JS Points" sheetId="3" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="291">
   <si>
     <t>Topics</t>
   </si>
@@ -1811,9 +1810,6 @@
     <t>Hoisting in Javascript</t>
   </si>
   <si>
-    <t>Removing duplicates from array?</t>
-  </si>
-  <si>
     <t>Pure component ?</t>
   </si>
   <si>
@@ -2119,12 +2115,6 @@
     <t xml:space="preserve">Explain virtual DOM. </t>
   </si>
   <si>
-    <t xml:space="preserve">Virtual Dom is a simple JavaScript object that is the exact copy of corresponding real DOM. 
-It can be considered as a node tree that consists of elements,their attributes and other properties. 
-Using the render function in react, it creates a node tree  and update its based on the changes that occurs in the data model. 
-This changes are usually triggered by users of the actions caused by the system. </t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -2179,12 +2169,160 @@
   <si>
     <t>Disadvantages of React</t>
   </si>
+  <si>
+    <t>Diff between state and variable</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Hoisting</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is JavaScript's default behavior of moving all declarations to the top of the current scope (to the top of the current script or the current function).                                        Variables defined with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>let</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>const</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> are hoisted to the top of the block, but not initialized </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(ReferenceError)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Virtual DOM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is a simple JavaScript object that is the exact copy of corresponding real DOM. 
+It can be considered as a node tree that consists of elements,their attributes and other properties. 
+Using the render function in react, it creates a node tree  and update its based on the changes that occurs in the data model. 
+This changes are usually triggered by users of the actions caused by the system. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Shallow copy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of an object create a new object and copies all the field of object to the new object (either it is primitive or a reference). In case of non-primitive types only reference will be copied to the new instance. Automatic changes the new object's value if old object change some value.                                                                    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Deep copy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of an object create a fully independent copy of an object. In case of deep copy everything will be copied to the new object.No changes occur in new object's value even after changing old objec'st value.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="29" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2394,6 +2532,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -2776,7 +2922,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2924,6 +3070,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3023,17 +3181,8 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3073,7 +3222,7 @@
         <xdr:cNvPr id="3" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4E2A9D0-6317-F80A-734A-BA487709DB1E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E4E2A9D0-6317-F80A-734A-BA487709DB1E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3142,7 +3291,7 @@
         <xdr:cNvPr id="4" name="Rectangle 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{460CD100-4C60-9655-E767-3F618142FBDC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{460CD100-4C60-9655-E767-3F618142FBDC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3267,7 +3416,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F0687AC-5F95-B371-FCC3-516ECEBB7F8D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4F0687AC-5F95-B371-FCC3-516ECEBB7F8D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3311,7 +3460,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38596EE9-12E8-E05D-656B-7E6C83468E69}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{38596EE9-12E8-E05D-656B-7E6C83468E69}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3355,7 +3504,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A44838A8-315A-6F11-F425-7C24684925CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A44838A8-315A-6F11-F425-7C24684925CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3399,7 +3548,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6468BF38-FF2D-C7D2-9142-120CFAF41A38}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6468BF38-FF2D-C7D2-9142-120CFAF41A38}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3443,7 +3592,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBCAADE1-0A65-E2AB-42C9-C833CC10A99A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EBCAADE1-0A65-E2AB-42C9-C833CC10A99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3491,7 +3640,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9A655E8-006A-EE32-F2F1-5080EB63AAF6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E9A655E8-006A-EE32-F2F1-5080EB63AAF6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3535,7 +3684,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA5A8967-9D46-7B4A-81EA-E5E7E0FBD1D4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FA5A8967-9D46-7B4A-81EA-E5E7E0FBD1D4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3579,7 +3728,7 @@
         <xdr:cNvPr id="10" name="Picture 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5628D44-680D-FB5E-E6FA-ECBA9934C1EE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D5628D44-680D-FB5E-E6FA-ECBA9934C1EE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3623,7 +3772,7 @@
         <xdr:cNvPr id="11" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7253AB4-994D-87AA-50A4-1E642115AF54}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E7253AB4-994D-87AA-50A4-1E642115AF54}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3667,7 +3816,7 @@
         <xdr:cNvPr id="12" name="Picture 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DDCCF8C-2871-9944-4A9D-EC8901C1674D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0DDCCF8C-2871-9944-4A9D-EC8901C1674D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3711,7 +3860,7 @@
         <xdr:cNvPr id="13" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D1A4CDE-62F4-A369-6F02-86865D0E6B72}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3D1A4CDE-62F4-A369-6F02-86865D0E6B72}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3760,7 +3909,7 @@
         <xdr:cNvPr id="2" name="Right Brace 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{271A39DF-730C-44C5-B2C6-BCC2EFAE8626}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{271A39DF-730C-44C5-B2C6-BCC2EFAE8626}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3838,7 +3987,7 @@
         <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5A86CCB-9035-382C-CB17-968C40DFAB49}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A5A86CCB-9035-382C-CB17-968C40DFAB49}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3888,7 +4037,7 @@
         <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5123DE96-BC07-92D0-1AEA-823B40633BA9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5123DE96-BC07-92D0-1AEA-823B40633BA9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3941,7 +4090,7 @@
         <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79B9A0D3-4108-418B-8375-3FDACBDFFF37}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{79B9A0D3-4108-418B-8375-3FDACBDFFF37}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3994,7 +4143,7 @@
         <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1073A0F4-BF25-49FD-B619-5EC5F802F813}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1073A0F4-BF25-49FD-B619-5EC5F802F813}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4047,7 +4196,7 @@
         <xdr:cNvPr id="11" name="Straight Connector 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{696E1177-F678-B27D-E168-36FA4288F520}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{696E1177-F678-B27D-E168-36FA4288F520}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4097,7 +4246,7 @@
         <xdr:cNvPr id="15" name="Straight Connector 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE6952BA-250D-47A8-9B95-78E49C76026E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AE6952BA-250D-47A8-9B95-78E49C76026E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4147,7 +4296,7 @@
         <xdr:cNvPr id="17" name="Connector: Elbow 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C26EC763-551C-C4BE-9443-748B6D540788}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C26EC763-551C-C4BE-9443-748B6D540788}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4205,7 +4354,7 @@
         <xdr:cNvPr id="20" name="Connector: Elbow 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{551A7CBE-D3B6-4E61-B697-B078049DE0AA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{551A7CBE-D3B6-4E61-B697-B078049DE0AA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4268,7 +4417,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4318,7 +4467,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4368,7 +4517,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4418,7 +4567,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4495,7 +4644,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4528,26 +4677,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4580,23 +4712,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4772,7 +4887,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D24"/>
   <sheetViews>
     <sheetView topLeftCell="A21" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -4792,10 +4907,10 @@
       <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="63" t="s">
         <v>3</v>
       </c>
     </row>
@@ -4803,8 +4918,8 @@
       <c r="B3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="60"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="64"/>
     </row>
     <row r="4" spans="2:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="52">
@@ -4876,18 +4991,18 @@
       <c r="B10" s="11">
         <v>7</v>
       </c>
-      <c r="C10" s="61" t="s">
+      <c r="C10" s="65" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
         <v>8</v>
       </c>
-      <c r="C11" s="62"/>
+      <c r="C11" s="66"/>
       <c r="D11" s="4" t="s">
         <v>18</v>
       </c>
@@ -4929,7 +5044,7 @@
       <c r="B15" s="2">
         <v>12</v>
       </c>
-      <c r="C15" s="63" t="s">
+      <c r="C15" s="67" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -4940,7 +5055,7 @@
       <c r="B16" s="2">
         <v>13</v>
       </c>
-      <c r="C16" s="63"/>
+      <c r="C16" s="67"/>
       <c r="D16" s="4" t="s">
         <v>25</v>
       </c>
@@ -5025,10 +5140,10 @@
         <v>21</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D24" s="43" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -5039,10 +5154,10 @@
     <mergeCell ref="C15:C16"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C19" location="' Array &amp; Object'!A1" display="What is Array ? " xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C21" location="' Array &amp; Object'!A1" display="JavaScript object. " xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C23" location="Operators!A1" display="JS Operators" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C24" location="'JS Error Types'!A1" display="Explain SyntaxError, ReferenceError and TypeError with examples" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C19" location="' Array &amp; Object'!A1" display="What is Array ? "/>
+    <hyperlink ref="C21" location="' Array &amp; Object'!A1" display="JavaScript object. "/>
+    <hyperlink ref="C23" location="Operators!A1" display="JS Operators"/>
+    <hyperlink ref="C24" location="'JS Error Types'!A1" display="Explain SyntaxError, ReferenceError and TypeError with examples"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5050,11 +5165,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5068,26 +5183,26 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="64" t="s">
-        <v>222</v>
-      </c>
-      <c r="D2" s="64" t="s">
+      <c r="C2" s="68" t="s">
+        <v>221</v>
+      </c>
+      <c r="D2" s="68" t="s">
         <v>3</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="64" t="s">
-        <v>221</v>
-      </c>
-      <c r="J2" s="64" t="s">
+      <c r="I2" s="68" t="s">
+        <v>220</v>
+      </c>
+      <c r="J2" s="68" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5095,13 +5210,13 @@
       <c r="B3" s="39" t="s">
         <v>206</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
       <c r="H3" s="39" t="s">
         <v>206</v>
       </c>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
@@ -5111,13 +5226,13 @@
         <v>207</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H4" s="2">
         <v>1</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J4" s="2"/>
     </row>
@@ -5126,16 +5241,16 @@
         <v>2</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D5" s="43" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H5" s="2">
         <v>2</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J5" s="2"/>
     </row>
@@ -5144,10 +5259,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="H6" s="2">
         <v>3</v>
@@ -5155,28 +5270,32 @@
       <c r="I6" s="3"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" s="94" t="s">
+        <v>288</v>
+      </c>
       <c r="H7" s="2">
         <v>4</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="D8" s="3"/>
+        <v>214</v>
+      </c>
+      <c r="D8" s="60" t="s">
+        <v>290</v>
+      </c>
       <c r="H8" s="2">
         <v>5</v>
       </c>
@@ -5202,7 +5321,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="D10" s="3"/>
       <c r="H10" s="2">
@@ -5211,29 +5330,31 @@
       <c r="I10" s="3"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
         <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="D11" s="3"/>
+        <v>277</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>289</v>
+      </c>
       <c r="H11" s="2">
         <v>8</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="B12" s="2">
         <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="D12" s="3" t="s">
         <v>279</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>280</v>
       </c>
       <c r="H12" s="2">
         <v>9</v>
@@ -5241,180 +5362,180 @@
       <c r="I12" s="3"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B13" s="2">
         <v>10</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="60" t="s">
         <v>282</v>
       </c>
-      <c r="H13" s="2">
-        <v>10</v>
-      </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="H13" s="57"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="57"/>
+    </row>
+    <row r="14" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="B14" s="2">
         <v>11</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="D14" s="60" t="s">
         <v>283</v>
       </c>
-      <c r="D14" s="93" t="s">
-        <v>284</v>
-      </c>
-      <c r="H14" s="90"/>
-      <c r="I14" s="91"/>
-      <c r="J14" s="90"/>
-    </row>
-    <row r="15" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="H14" s="57"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="57"/>
+    </row>
+    <row r="15" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B15" s="2">
         <v>12</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="D15" s="93" t="s">
+      <c r="D15" s="60" t="s">
         <v>285</v>
       </c>
-      <c r="H15" s="90"/>
-      <c r="I15" s="91"/>
-      <c r="J15" s="90"/>
-    </row>
-    <row r="16" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="H15" s="57"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="57"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <v>13</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="D16" s="93" t="s">
-        <v>287</v>
-      </c>
-      <c r="H16" s="90"/>
-      <c r="I16" s="91"/>
-      <c r="J16" s="90"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="60"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="57"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="2">
         <v>14</v>
       </c>
       <c r="C17" s="3"/>
-      <c r="D17" s="93"/>
-      <c r="H17" s="90"/>
-      <c r="I17" s="91"/>
-      <c r="J17" s="90"/>
+      <c r="D17" s="60"/>
+      <c r="H17" s="57"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="57"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="2">
         <v>15</v>
       </c>
       <c r="C18" s="3"/>
-      <c r="D18" s="93"/>
-      <c r="H18" s="90"/>
-      <c r="I18" s="91"/>
-      <c r="J18" s="90"/>
+      <c r="D18" s="60"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="57"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="2">
         <v>16</v>
       </c>
       <c r="C19" s="3"/>
-      <c r="D19" s="93"/>
-      <c r="H19" s="90"/>
-      <c r="I19" s="91"/>
-      <c r="J19" s="90"/>
+      <c r="D19" s="60"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="57"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" s="2">
         <v>17</v>
       </c>
       <c r="C20" s="3"/>
-      <c r="D20" s="93"/>
-      <c r="H20" s="90"/>
-      <c r="I20" s="91"/>
-      <c r="J20" s="90"/>
+      <c r="D20" s="60"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="57"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B21" s="2">
-        <v>18</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="93"/>
-      <c r="H21" s="90"/>
-      <c r="I21" s="91"/>
-      <c r="J21" s="90"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B22" s="90"/>
-      <c r="C22" s="91"/>
-      <c r="D22" s="92"/>
-      <c r="H22" s="90"/>
-      <c r="I22" s="91"/>
-      <c r="J22" s="90"/>
-    </row>
-    <row r="26" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B26" s="11" t="s">
+      <c r="B21" s="57"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="59"/>
+      <c r="H21" s="57"/>
+      <c r="I21" s="58"/>
+      <c r="J21" s="57"/>
+    </row>
+    <row r="25" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B25" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C26" s="64" t="s">
-        <v>214</v>
-      </c>
-      <c r="D26" s="64" t="s">
+      <c r="C25" s="68" t="s">
+        <v>213</v>
+      </c>
+      <c r="D25" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="H26" s="11" t="s">
+      <c r="H25" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I26" s="64" t="s">
+      <c r="I25" s="68" t="s">
+        <v>226</v>
+      </c>
+      <c r="J25" s="68" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="B26" s="39" t="s">
+        <v>206</v>
+      </c>
+      <c r="C26" s="68"/>
+      <c r="D26" s="68"/>
+      <c r="H26" s="39" t="s">
+        <v>206</v>
+      </c>
+      <c r="I26" s="68"/>
+      <c r="J26" s="68"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B27" s="2">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="H27" s="2">
+        <v>1</v>
+      </c>
+      <c r="I27" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="J26" s="64" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="B27" s="39" t="s">
-        <v>206</v>
-      </c>
-      <c r="C27" s="64"/>
-      <c r="D27" s="64"/>
-      <c r="H27" s="39" t="s">
-        <v>206</v>
-      </c>
-      <c r="I27" s="64"/>
-      <c r="J27" s="64"/>
+      <c r="J27" s="2"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B28" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>210</v>
       </c>
       <c r="D28" s="3"/>
       <c r="H28" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>228</v>
       </c>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B29" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>211</v>
       </c>
       <c r="D29" s="3"/>
       <c r="H29" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I29" s="3" t="s">
         <v>229</v>
@@ -5423,14 +5544,14 @@
     </row>
     <row r="30" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B30" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>212</v>
       </c>
       <c r="D30" s="3"/>
       <c r="H30" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I30" s="3" t="s">
         <v>230</v>
@@ -5439,14 +5560,14 @@
     </row>
     <row r="31" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B31" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D31" s="3"/>
       <c r="H31" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I31" s="3" t="s">
         <v>231</v>
@@ -5455,191 +5576,177 @@
     </row>
     <row r="32" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B32" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>217</v>
       </c>
       <c r="D32" s="3"/>
       <c r="H32" s="2">
-        <v>5</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>232</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="I32" s="3"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B33" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="D33" s="3"/>
       <c r="H33" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I33" s="3"/>
       <c r="J33" s="2"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B34" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>223</v>
       </c>
       <c r="D34" s="3"/>
       <c r="H34" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I34" s="3"/>
       <c r="J34" s="2"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B35" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>224</v>
+        <v>287</v>
       </c>
       <c r="D35" s="3"/>
       <c r="H35" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I35" s="3"/>
       <c r="J35" s="2"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B36" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="H36" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I36" s="3"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B37" s="2">
-        <v>10</v>
-      </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="H37" s="2">
-        <v>10</v>
-      </c>
-      <c r="I37" s="3"/>
-      <c r="J37" s="2"/>
-    </row>
-    <row r="40" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B40" s="11" t="s">
+    <row r="39" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B39" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C40" s="64" t="s">
+      <c r="C39" s="68" t="s">
+        <v>232</v>
+      </c>
+      <c r="D39" s="68" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="B40" s="39" t="s">
+        <v>206</v>
+      </c>
+      <c r="C40" s="68"/>
+      <c r="D40" s="68"/>
+    </row>
+    <row r="41" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B41" s="2">
+        <v>1</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="D40" s="64" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="B41" s="39" t="s">
-        <v>206</v>
-      </c>
-      <c r="C41" s="64"/>
-      <c r="D41" s="64"/>
-    </row>
-    <row r="42" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B42" s="2">
-        <v>1</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>234</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B43" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B44" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B45" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B46" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B47" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B48" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B51" s="2">
-        <v>10</v>
-      </c>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-    </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
     <mergeCell ref="I2:I3"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="J25:J26"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C5" location="'JS Error Types'!A1" display="Explain Type Error, Syntax Error and Referrence Error" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="C5" location="'JS Error Types'!A1" display="Explain Type Error, Syntax Error and Referrence Error"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5648,7 +5755,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5789,10 +5896,10 @@
         <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>247</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
@@ -5800,10 +5907,10 @@
         <v>12</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>249</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
@@ -5811,10 +5918,10 @@
         <v>13</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>251</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -5822,10 +5929,10 @@
         <v>14</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>253</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -5833,10 +5940,10 @@
         <v>15</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>255</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -5844,10 +5951,10 @@
         <v>16</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>257</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -5855,10 +5962,10 @@
         <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>259</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -5866,10 +5973,10 @@
         <v>18</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>261</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="158.4" x14ac:dyDescent="0.3">
@@ -5877,10 +5984,10 @@
         <v>19</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>263</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="158.4" x14ac:dyDescent="0.3">
@@ -5888,10 +5995,10 @@
         <v>20</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>265</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -5899,10 +6006,10 @@
         <v>21</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>267</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -5910,10 +6017,10 @@
         <v>22</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>269</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -5921,10 +6028,10 @@
         <v>23</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>271</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
@@ -5932,10 +6039,10 @@
         <v>24</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>273</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
@@ -5943,10 +6050,10 @@
         <v>25</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>275</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="28" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -5954,7 +6061,7 @@
         <v>26</v>
       </c>
       <c r="C28" s="40" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -5963,7 +6070,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5985,10 +6092,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="68"/>
+      <c r="C3" s="72"/>
       <c r="D3" s="15" t="s">
         <v>69</v>
       </c>
@@ -6000,10 +6107,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="69"/>
+      <c r="C4" s="73"/>
       <c r="D4" s="2" t="s">
         <v>73</v>
       </c>
@@ -6015,16 +6122,16 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="74" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="61" t="s">
+      <c r="C5" s="65" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="65" t="s">
+      <c r="D5" s="69" t="s">
         <v>78</v>
       </c>
-      <c r="E5" s="65" t="s">
+      <c r="E5" s="69" t="s">
         <v>78</v>
       </c>
       <c r="F5" s="14" t="s">
@@ -6032,16 +6139,16 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="70"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
       <c r="F6" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B7" s="70"/>
+      <c r="B7" s="74"/>
       <c r="C7" s="14" t="s">
         <v>81</v>
       </c>
@@ -6056,7 +6163,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B8" s="70"/>
+      <c r="B8" s="74"/>
       <c r="C8" s="14" t="s">
         <v>85</v>
       </c>
@@ -6071,7 +6178,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="B9" s="70"/>
+      <c r="B9" s="74"/>
       <c r="C9" s="14" t="s">
         <v>89</v>
       </c>
@@ -6082,7 +6189,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="B10" s="70"/>
+      <c r="B10" s="74"/>
       <c r="C10" s="14" t="s">
         <v>91</v>
       </c>
@@ -6093,7 +6200,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="70"/>
+      <c r="B11" s="74"/>
       <c r="C11" s="14" t="s">
         <v>93</v>
       </c>
@@ -6106,10 +6213,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B12" s="67" t="s">
+      <c r="B12" s="71" t="s">
         <v>96</v>
       </c>
-      <c r="C12" s="67"/>
+      <c r="C12" s="71"/>
       <c r="D12" s="4" t="s">
         <v>97</v>
       </c>
@@ -6131,14 +6238,14 @@
     <mergeCell ref="C5:C6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Js points'!A1" display="Back to main page" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="A1" location="'Js points'!A1" display="Back to main page"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6152,10 +6259,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="71"/>
+      <c r="C2" s="75"/>
     </row>
     <row r="3" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="30" t="s">
@@ -6434,39 +6541,39 @@
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" display="https://www.w3schools.com/JSREF/jsref_concat_array.asp" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="B5" r:id="rId2" display="https://www.w3schools.com/JSREF/jsref_constructor_array.asp" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="B6" r:id="rId3" display="https://www.w3schools.com/JSREF/jsref_copywithin.asp" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
-    <hyperlink ref="B7" r:id="rId4" display="https://www.w3schools.com/JSREF/jsref_entries.asp" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
-    <hyperlink ref="B8" r:id="rId5" display="https://www.w3schools.com/JSREF/jsref_every.asp" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
-    <hyperlink ref="B9" r:id="rId6" display="https://www.w3schools.com/JSREF/jsref_fill.asp" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
-    <hyperlink ref="B10" r:id="rId7" display="https://www.w3schools.com/JSREF/jsref_filter.asp" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
-    <hyperlink ref="B11" r:id="rId8" display="https://www.w3schools.com/JSREF/jsref_find.asp" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
-    <hyperlink ref="B12" r:id="rId9" display="https://www.w3schools.com/JSREF/jsref_findindex.asp" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
-    <hyperlink ref="B13" r:id="rId10" display="https://www.w3schools.com/JSREF/jsref_foreach.asp" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
-    <hyperlink ref="B14" r:id="rId11" display="https://www.w3schools.com/JSREF/jsref_from.asp" xr:uid="{00000000-0004-0000-0400-00000A000000}"/>
-    <hyperlink ref="B15" r:id="rId12" display="https://www.w3schools.com/JSREF/jsref_includes_array.asp" xr:uid="{00000000-0004-0000-0400-00000B000000}"/>
-    <hyperlink ref="B16" r:id="rId13" display="https://www.w3schools.com/JSREF/jsref_indexof_array.asp" xr:uid="{00000000-0004-0000-0400-00000C000000}"/>
-    <hyperlink ref="B17" r:id="rId14" display="https://www.w3schools.com/JSREF/jsref_isarray.asp" xr:uid="{00000000-0004-0000-0400-00000D000000}"/>
-    <hyperlink ref="B18" r:id="rId15" display="https://www.w3schools.com/JSREF/jsref_join.asp" xr:uid="{00000000-0004-0000-0400-00000E000000}"/>
-    <hyperlink ref="B19" r:id="rId16" display="https://www.w3schools.com/JSREF/jsref_keys.asp" xr:uid="{00000000-0004-0000-0400-00000F000000}"/>
-    <hyperlink ref="B20" r:id="rId17" display="https://www.w3schools.com/JSREF/jsref_lastindexof_array.asp" xr:uid="{00000000-0004-0000-0400-000010000000}"/>
-    <hyperlink ref="B21" r:id="rId18" display="https://www.w3schools.com/JSREF/jsref_length_array.asp" xr:uid="{00000000-0004-0000-0400-000011000000}"/>
-    <hyperlink ref="B22" r:id="rId19" display="https://www.w3schools.com/JSREF/jsref_map.asp" xr:uid="{00000000-0004-0000-0400-000012000000}"/>
-    <hyperlink ref="B23" r:id="rId20" display="https://www.w3schools.com/JSREF/jsref_pop.asp" xr:uid="{00000000-0004-0000-0400-000013000000}"/>
-    <hyperlink ref="B24" r:id="rId21" display="https://www.w3schools.com/JSREF/jsref_prototype_array.asp" xr:uid="{00000000-0004-0000-0400-000014000000}"/>
-    <hyperlink ref="B25" r:id="rId22" display="https://www.w3schools.com/JSREF/jsref_push.asp" xr:uid="{00000000-0004-0000-0400-000015000000}"/>
-    <hyperlink ref="B26" r:id="rId23" display="https://www.w3schools.com/JSREF/jsref_reduce.asp" xr:uid="{00000000-0004-0000-0400-000016000000}"/>
-    <hyperlink ref="B27" r:id="rId24" display="https://www.w3schools.com/JSREF/jsref_reduceright.asp" xr:uid="{00000000-0004-0000-0400-000017000000}"/>
-    <hyperlink ref="B28" r:id="rId25" display="https://www.w3schools.com/JSREF/jsref_reverse.asp" xr:uid="{00000000-0004-0000-0400-000018000000}"/>
-    <hyperlink ref="B29" r:id="rId26" display="https://www.w3schools.com/JSREF/jsref_shift.asp" xr:uid="{00000000-0004-0000-0400-000019000000}"/>
-    <hyperlink ref="B30" r:id="rId27" display="https://www.w3schools.com/JSREF/jsref_slice_array.asp" xr:uid="{00000000-0004-0000-0400-00001A000000}"/>
-    <hyperlink ref="B31" r:id="rId28" display="https://www.w3schools.com/JSREF/jsref_some.asp" xr:uid="{00000000-0004-0000-0400-00001B000000}"/>
-    <hyperlink ref="B32" r:id="rId29" display="https://www.w3schools.com/JSREF/jsref_sort.asp" xr:uid="{00000000-0004-0000-0400-00001C000000}"/>
-    <hyperlink ref="B33" r:id="rId30" display="https://www.w3schools.com/JSREF/jsref_splice.asp" xr:uid="{00000000-0004-0000-0400-00001D000000}"/>
-    <hyperlink ref="B34" r:id="rId31" display="https://www.w3schools.com/JSREF/jsref_tostring_array.asp" xr:uid="{00000000-0004-0000-0400-00001E000000}"/>
-    <hyperlink ref="B35" r:id="rId32" display="https://www.w3schools.com/JSREF/jsref_unshift.asp" xr:uid="{00000000-0004-0000-0400-00001F000000}"/>
-    <hyperlink ref="B36" r:id="rId33" display="https://www.w3schools.com/JSREF/jsref_valueof_array.asp" xr:uid="{00000000-0004-0000-0400-000020000000}"/>
+    <hyperlink ref="B4" r:id="rId1" display="https://www.w3schools.com/JSREF/jsref_concat_array.asp"/>
+    <hyperlink ref="B5" r:id="rId2" display="https://www.w3schools.com/JSREF/jsref_constructor_array.asp"/>
+    <hyperlink ref="B6" r:id="rId3" display="https://www.w3schools.com/JSREF/jsref_copywithin.asp"/>
+    <hyperlink ref="B7" r:id="rId4" display="https://www.w3schools.com/JSREF/jsref_entries.asp"/>
+    <hyperlink ref="B8" r:id="rId5" display="https://www.w3schools.com/JSREF/jsref_every.asp"/>
+    <hyperlink ref="B9" r:id="rId6" display="https://www.w3schools.com/JSREF/jsref_fill.asp"/>
+    <hyperlink ref="B10" r:id="rId7" display="https://www.w3schools.com/JSREF/jsref_filter.asp"/>
+    <hyperlink ref="B11" r:id="rId8" display="https://www.w3schools.com/JSREF/jsref_find.asp"/>
+    <hyperlink ref="B12" r:id="rId9" display="https://www.w3schools.com/JSREF/jsref_findindex.asp"/>
+    <hyperlink ref="B13" r:id="rId10" display="https://www.w3schools.com/JSREF/jsref_foreach.asp"/>
+    <hyperlink ref="B14" r:id="rId11" display="https://www.w3schools.com/JSREF/jsref_from.asp"/>
+    <hyperlink ref="B15" r:id="rId12" display="https://www.w3schools.com/JSREF/jsref_includes_array.asp"/>
+    <hyperlink ref="B16" r:id="rId13" display="https://www.w3schools.com/JSREF/jsref_indexof_array.asp"/>
+    <hyperlink ref="B17" r:id="rId14" display="https://www.w3schools.com/JSREF/jsref_isarray.asp"/>
+    <hyperlink ref="B18" r:id="rId15" display="https://www.w3schools.com/JSREF/jsref_join.asp"/>
+    <hyperlink ref="B19" r:id="rId16" display="https://www.w3schools.com/JSREF/jsref_keys.asp"/>
+    <hyperlink ref="B20" r:id="rId17" display="https://www.w3schools.com/JSREF/jsref_lastindexof_array.asp"/>
+    <hyperlink ref="B21" r:id="rId18" display="https://www.w3schools.com/JSREF/jsref_length_array.asp"/>
+    <hyperlink ref="B22" r:id="rId19" display="https://www.w3schools.com/JSREF/jsref_map.asp"/>
+    <hyperlink ref="B23" r:id="rId20" display="https://www.w3schools.com/JSREF/jsref_pop.asp"/>
+    <hyperlink ref="B24" r:id="rId21" display="https://www.w3schools.com/JSREF/jsref_prototype_array.asp"/>
+    <hyperlink ref="B25" r:id="rId22" display="https://www.w3schools.com/JSREF/jsref_push.asp"/>
+    <hyperlink ref="B26" r:id="rId23" display="https://www.w3schools.com/JSREF/jsref_reduce.asp"/>
+    <hyperlink ref="B27" r:id="rId24" display="https://www.w3schools.com/JSREF/jsref_reduceright.asp"/>
+    <hyperlink ref="B28" r:id="rId25" display="https://www.w3schools.com/JSREF/jsref_reverse.asp"/>
+    <hyperlink ref="B29" r:id="rId26" display="https://www.w3schools.com/JSREF/jsref_shift.asp"/>
+    <hyperlink ref="B30" r:id="rId27" display="https://www.w3schools.com/JSREF/jsref_slice_array.asp"/>
+    <hyperlink ref="B31" r:id="rId28" display="https://www.w3schools.com/JSREF/jsref_some.asp"/>
+    <hyperlink ref="B32" r:id="rId29" display="https://www.w3schools.com/JSREF/jsref_sort.asp"/>
+    <hyperlink ref="B33" r:id="rId30" display="https://www.w3schools.com/JSREF/jsref_splice.asp"/>
+    <hyperlink ref="B34" r:id="rId31" display="https://www.w3schools.com/JSREF/jsref_tostring_array.asp"/>
+    <hyperlink ref="B35" r:id="rId32" display="https://www.w3schools.com/JSREF/jsref_unshift.asp"/>
+    <hyperlink ref="B36" r:id="rId33" display="https://www.w3schools.com/JSREF/jsref_valueof_array.asp"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId34"/>
@@ -6474,7 +6581,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView topLeftCell="A5" zoomScaleNormal="100" zoomScaleSheetLayoutView="11" workbookViewId="0">
@@ -6508,9 +6615,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink ref="A1" location="'Js points'!A1" display="Back to main FILE" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="A1" location="'Js points'!A1" display="Back to main FILE"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -6519,7 +6626,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E22"/>
   <sheetViews>
     <sheetView topLeftCell="C20" workbookViewId="0">
@@ -6539,10 +6646,10 @@
       <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="64" t="s">
+      <c r="D2" s="68" t="s">
         <v>3</v>
       </c>
     </row>
@@ -6550,8 +6657,8 @@
       <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
     </row>
     <row r="4" spans="2:5" ht="294.60000000000002" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
@@ -6602,7 +6709,7 @@
       <c r="B8" s="2">
         <v>5</v>
       </c>
-      <c r="C8" s="61" t="s">
+      <c r="C8" s="65" t="s">
         <v>33</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -6613,7 +6720,7 @@
       <c r="B9" s="2">
         <v>6</v>
       </c>
-      <c r="C9" s="62"/>
+      <c r="C9" s="66"/>
       <c r="D9" s="4" t="s">
         <v>36</v>
       </c>
@@ -6774,7 +6881,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6791,16 +6898,16 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="44" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:13" s="45" customFormat="1" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B3" s="81" t="s">
-        <v>240</v>
-      </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="83"/>
+      <c r="B3" s="85" t="s">
+        <v>239</v>
+      </c>
+      <c r="C3" s="86"/>
+      <c r="D3" s="87"/>
       <c r="E3" s="46"/>
       <c r="F3" s="46"/>
       <c r="G3" s="46"/>
@@ -6812,11 +6919,11 @@
       <c r="M3" s="46"/>
     </row>
     <row r="4" spans="1:13" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="84" t="s">
-        <v>241</v>
-      </c>
-      <c r="C4" s="85"/>
-      <c r="D4" s="86"/>
+      <c r="B4" s="88" t="s">
+        <v>240</v>
+      </c>
+      <c r="C4" s="89"/>
+      <c r="D4" s="90"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5" s="47"/>
@@ -6907,21 +7014,21 @@
       <c r="D26" s="48"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B27" s="75"/>
-      <c r="C27" s="76"/>
-      <c r="D27" s="77"/>
+      <c r="B27" s="79"/>
+      <c r="C27" s="80"/>
+      <c r="D27" s="81"/>
     </row>
     <row r="28" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="78"/>
-      <c r="C28" s="79"/>
-      <c r="D28" s="80"/>
+      <c r="B28" s="82"/>
+      <c r="C28" s="83"/>
+      <c r="D28" s="84"/>
     </row>
     <row r="29" spans="2:4" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B29" s="87" t="s">
-        <v>242</v>
-      </c>
-      <c r="C29" s="88"/>
-      <c r="D29" s="89"/>
+      <c r="B29" s="91" t="s">
+        <v>241</v>
+      </c>
+      <c r="C29" s="92"/>
+      <c r="D29" s="93"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" s="47"/>
@@ -7004,21 +7111,21 @@
       <c r="D49" s="48"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B50" s="75"/>
-      <c r="C50" s="76"/>
-      <c r="D50" s="77"/>
+      <c r="B50" s="79"/>
+      <c r="C50" s="80"/>
+      <c r="D50" s="81"/>
     </row>
     <row r="51" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="78"/>
-      <c r="C51" s="79"/>
-      <c r="D51" s="80"/>
+      <c r="B51" s="82"/>
+      <c r="C51" s="83"/>
+      <c r="D51" s="84"/>
     </row>
     <row r="52" spans="2:4" ht="24" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="72" t="s">
-        <v>243</v>
-      </c>
-      <c r="C52" s="73"/>
-      <c r="D52" s="74"/>
+      <c r="B52" s="76" t="s">
+        <v>242</v>
+      </c>
+      <c r="C52" s="77"/>
+      <c r="D52" s="78"/>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B53" s="47"/>
@@ -7101,26 +7208,26 @@
       <c r="D72" s="48"/>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B73" s="75"/>
-      <c r="C73" s="76"/>
-      <c r="D73" s="77"/>
+      <c r="B73" s="79"/>
+      <c r="C73" s="80"/>
+      <c r="D73" s="81"/>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B74" s="75"/>
-      <c r="C74" s="76"/>
-      <c r="D74" s="77"/>
+      <c r="B74" s="79"/>
+      <c r="C74" s="80"/>
+      <c r="D74" s="81"/>
     </row>
     <row r="75" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B75" s="78"/>
-      <c r="C75" s="79"/>
-      <c r="D75" s="80"/>
+      <c r="B75" s="82"/>
+      <c r="C75" s="83"/>
+      <c r="D75" s="84"/>
     </row>
     <row r="76" spans="2:4" ht="24" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B76" s="72" t="s">
-        <v>244</v>
-      </c>
-      <c r="C76" s="73"/>
-      <c r="D76" s="74"/>
+      <c r="B76" s="76" t="s">
+        <v>243</v>
+      </c>
+      <c r="C76" s="77"/>
+      <c r="D76" s="78"/>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B77" s="47"/>
@@ -7175,8 +7282,8 @@
     <mergeCell ref="B52:D52"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" location="'JS Points'!A1" display="Back To Home" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="A1" location="'JS Points'!A1" display="Back To Home"/>
+    <hyperlink ref="B3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>

</xml_diff>